<commit_message>
Vendor Invoice details changes
</commit_message>
<xml_diff>
--- a/WppRegPack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
+++ b/WppRegPack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="10" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -1958,10 +1958,10 @@
     <t>1307100097</t>
   </si>
   <si>
-    <t>a13071000732</t>
-  </si>
-  <si>
     <t>MA1307235H</t>
+  </si>
+  <si>
+    <t>ab13071000732</t>
   </si>
 </sst>
 </file>
@@ -3882,7 +3882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -3961,7 +3961,7 @@
         <v>555</v>
       </c>
       <c r="B9" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4363,7 +4363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -4420,10 +4420,10 @@
         <v>1307</v>
       </c>
       <c r="C2" s="67" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="D2" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
   </sheetData>

</xml_diff>